<commit_message>
adjust noise power filter
</commit_message>
<xml_diff>
--- a/Power_Filter_IIR_calc.xlsx
+++ b/Power_Filter_IIR_calc.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440"/>
   </bookViews>
   <sheets>
-    <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
+    <sheet name="Signal Power Filter" sheetId="5" r:id="rId1"/>
+    <sheet name="Noise Power Filter" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>cutoff freq</t>
   </si>
@@ -470,7 +471,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -480,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -502,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -513,7 +514,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -525,7 +526,7 @@
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>62.831853071795862</v>
+        <v>628.31853071795865</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -537,7 +538,7 @@
       </c>
       <c r="B5">
         <f>1/B3</f>
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -552,7 +553,7 @@
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>64.983939246581258</v>
+        <v>649.83939246581258</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -683,6 +684,227 @@
       <c r="B22" s="1">
         <f>ROUND(B19*B12,0)</f>
         <v>16696</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>2*PI()*B2</f>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>1/B3</f>
+        <v>1E-3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>(2*B3)*TAN(B4*B5/2)</f>
+        <v>6.2832059781123126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>B6*B5</f>
+        <v>6.2832059781123125E-3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>2+(B8)</f>
+        <v>2.0062832059781122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>2-B8</f>
+        <v>1.9937167940218876</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>B10/B9</f>
+        <v>0.9937364715416146</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <f>B8/B9</f>
+        <v>3.1317642291927056E-3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <f>B8/B9</f>
+        <v>3.1317642291927056E-3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <f>POWER(2,B18)</f>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <f>ROUND(B19*B13*B16,0)</f>
+        <v>103</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1">
+        <f>ROUND(B19*B14*B16,0)</f>
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="1">
+        <f>ROUND(B19*B12,0)</f>
+        <v>32563</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>

</xml_diff>